<commit_message>
Slight change to ISA
</commit_message>
<xml_diff>
--- a/Documentation/ISA.xlsx
+++ b/Documentation/ISA.xlsx
@@ -131,9 +131,6 @@
     <t>JTS</t>
   </si>
   <si>
-    <t>JSR n</t>
-  </si>
-  <si>
     <t>Jump to subroutine n</t>
   </si>
   <si>
@@ -236,18 +233,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>STDM</t>
-  </si>
-  <si>
-    <t>LDDM</t>
-  </si>
-  <si>
-    <t>LDDM Rd,[n]</t>
-  </si>
-  <si>
-    <t>STDM [n],Rs</t>
-  </si>
-  <si>
     <t>[n] &lt;- Rs</t>
   </si>
   <si>
@@ -377,21 +362,12 @@
     <t>Rd &lt;- Rd OR Rs</t>
   </si>
   <si>
-    <t>LDX</t>
-  </si>
-  <si>
-    <t>LDX Rd,[Rs]</t>
-  </si>
-  <si>
     <t>Indirect load from data memory</t>
   </si>
   <si>
     <t>Rd &lt;- [Rs]</t>
   </si>
   <si>
-    <t>STX</t>
-  </si>
-  <si>
     <t>Direct load from data memory</t>
   </si>
   <si>
@@ -401,9 +377,6 @@
     <t>Direct store to data memory</t>
   </si>
   <si>
-    <t>STX [Rd],Rs</t>
-  </si>
-  <si>
     <t>[Rd] &lt;- Rs</t>
   </si>
   <si>
@@ -579,6 +552,33 @@
   </si>
   <si>
     <t>PC &lt;- N ? n : PC+1</t>
+  </si>
+  <si>
+    <t>JTS n</t>
+  </si>
+  <si>
+    <t>LDD</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>LID</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>LID Rd,[Rs]</t>
+  </si>
+  <si>
+    <t>SIT [Rd],Rs</t>
+  </si>
+  <si>
+    <t>LDD Rd,[n]</t>
+  </si>
+  <si>
+    <t>STD [n],Rs</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1177,7 @@
   <dimension ref="A3:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1201,7 @@
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -1210,7 +1210,7 @@
       <c r="G3" s="28"/>
       <c r="H3" s="29"/>
       <c r="I3" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
@@ -1228,7 +1228,7 @@
       <c r="W3" s="37"/>
       <c r="X3" s="38"/>
       <c r="Z3" s="42" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AA3" s="43"/>
       <c r="AB3" s="20"/>
@@ -1270,14 +1270,14 @@
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="I5" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5" s="48"/>
       <c r="K5" s="48"/>
       <c r="L5" s="48"/>
       <c r="M5" s="49"/>
       <c r="N5" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O5" s="48"/>
       <c r="P5" s="48"/>
@@ -1372,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="AB6" s="10"/>
     </row>
@@ -1448,10 +1448,10 @@
         <v>22</v>
       </c>
       <c r="Z7" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA7" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="AB7" s="10"/>
     </row>
@@ -1527,10 +1527,10 @@
         <v>22</v>
       </c>
       <c r="Z8" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="AA8" s="20" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="AB8" s="10"/>
     </row>
@@ -1606,10 +1606,10 @@
         <v>22</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AA9" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1618,19 +1618,19 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2">
         <v>2</v>
@@ -1690,19 +1690,19 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H11" s="2">
         <v>2</v>
@@ -1765,16 +1765,16 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H12" s="2">
         <v>2</v>
@@ -1804,31 +1804,31 @@
         <v>21</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z12" s="42" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="AA12" s="43"/>
     </row>
@@ -1838,19 +1838,19 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H13" s="2">
         <v>2</v>
@@ -1990,19 +1990,19 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H15" s="2">
         <v>3</v>
@@ -2023,13 +2023,13 @@
         <v>28</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q15" s="5" t="s">
         <v>22</v>
@@ -2056,10 +2056,10 @@
         <v>22</v>
       </c>
       <c r="Z15" s="19" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="AA15" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -2068,19 +2068,19 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="H16" s="2">
         <v>3</v>
@@ -2101,13 +2101,13 @@
         <v>33</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="5" t="s">
         <v>22</v>
@@ -2134,31 +2134,31 @@
         <v>22</v>
       </c>
       <c r="Z16" s="19" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="AA16" s="17" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H17" s="2">
         <v>3</v>
@@ -2179,13 +2179,13 @@
         <v>28</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>22</v>
@@ -2213,31 +2213,31 @@
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="19" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="AA17" s="17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H18" s="2">
         <v>3</v>
@@ -2258,13 +2258,13 @@
         <v>33</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>22</v>
@@ -2292,31 +2292,31 @@
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="21" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="AA18" s="22" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H19" s="2">
         <v>2</v>
@@ -2337,13 +2337,13 @@
         <v>28</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q19" s="5" t="s">
         <v>22</v>
@@ -2374,22 +2374,22 @@
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H20" s="2">
         <v>2</v>
@@ -2410,13 +2410,13 @@
         <v>33</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>22</v>
@@ -2447,22 +2447,22 @@
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>73</v>
+        <v>184</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H21" s="2">
         <v>2</v>
@@ -2483,13 +2483,13 @@
         <v>28</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>22</v>
@@ -2517,29 +2517,29 @@
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="42" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="AA21" s="43"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="H22" s="2">
         <v>2</v>
@@ -2560,13 +2560,13 @@
         <v>33</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>21</v>
@@ -2599,22 +2599,22 @@
     <row r="23" spans="1:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H23" s="2">
         <v>2</v>
@@ -2635,22 +2635,22 @@
         <v>28</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T23" s="5" t="s">
         <v>21</v>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="25" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="AA23" s="26" t="s">
         <v>2</v>
@@ -2678,22 +2678,22 @@
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H24" s="2">
         <v>2</v>
@@ -2714,22 +2714,22 @@
         <v>33</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T24" s="5" t="s">
         <v>21</v>
@@ -2748,31 +2748,31 @@
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="19" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="AA24" s="17" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H25" s="2">
         <v>2</v>
@@ -2793,22 +2793,22 @@
         <v>28</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T25" s="5" t="s">
         <v>21</v>
@@ -2827,31 +2827,31 @@
       </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="19" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="AA25" s="17" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H26" s="2">
         <v>2</v>
@@ -2872,22 +2872,22 @@
         <v>33</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S26" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T26" s="5" t="s">
         <v>21</v>
@@ -2906,31 +2906,31 @@
       </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="19" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="AA26" s="17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>118</v>
+        <v>181</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H27" s="2">
         <v>2</v>
@@ -2951,22 +2951,22 @@
         <v>28</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T27" s="5" t="s">
         <v>21</v>
@@ -2985,31 +2985,31 @@
       </c>
       <c r="Y27" s="10"/>
       <c r="Z27" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA27" s="17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>121</v>
+        <v>180</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="H28" s="2">
         <v>2</v>
@@ -3030,22 +3030,22 @@
         <v>33</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T28" s="5" t="s">
         <v>21</v>
@@ -3064,31 +3064,31 @@
       </c>
       <c r="Y28" s="10"/>
       <c r="Z28" s="21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="AA28" s="22" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="H29" s="2">
         <v>2</v>
@@ -3109,13 +3109,13 @@
         <v>28</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="Q29" s="5" t="s">
         <v>21</v>
@@ -3146,22 +3146,22 @@
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="H30" s="2">
         <v>3</v>
@@ -3182,13 +3182,13 @@
         <v>33</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q30" s="5" t="s">
         <v>21</v>
@@ -3219,7 +3219,7 @@
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>21</v>
@@ -3255,13 +3255,13 @@
         <v>28</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q31" s="5" t="s">
         <v>21</v>
@@ -3292,22 +3292,22 @@
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H32" s="2">
         <v>2</v>
@@ -3328,13 +3328,13 @@
         <v>33</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q32" s="5" t="s">
         <v>21</v>
@@ -3365,22 +3365,22 @@
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H33" s="2">
         <v>2</v>
@@ -3401,13 +3401,13 @@
         <v>28</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q33" s="5" t="s">
         <v>21</v>
@@ -3438,22 +3438,22 @@
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H34" s="2">
         <v>2</v>
@@ -3474,13 +3474,13 @@
         <v>33</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="P34" s="5" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="Q34" s="5" t="s">
         <v>21</v>
@@ -3511,7 +3511,7 @@
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>21</v>
@@ -3584,7 +3584,7 @@
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>21</v>
@@ -3657,22 +3657,22 @@
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H37" s="2">
         <v>2</v>
@@ -3730,19 +3730,19 @@
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Updated ISA and added an ASM example
</commit_message>
<xml_diff>
--- a/Documentation/ISA.xlsx
+++ b/Documentation/ISA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Subarashii-CPU\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\Subarashii-CPU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="182">
   <si>
     <t>Index</t>
   </si>
@@ -473,15 +473,6 @@
     <t>Halt processor</t>
   </si>
   <si>
-    <t>RST</t>
-  </si>
-  <si>
-    <t>PC &lt;- 0</t>
-  </si>
-  <si>
-    <t>Reset processor</t>
-  </si>
-  <si>
     <t>Instruction Types</t>
   </si>
   <si>
@@ -566,19 +557,19 @@
     <t>LID</t>
   </si>
   <si>
-    <t>SIT</t>
-  </si>
-  <si>
     <t>LID Rd,[Rs]</t>
   </si>
   <si>
-    <t>SIT [Rd],Rs</t>
-  </si>
-  <si>
     <t>LDD Rd,[n]</t>
   </si>
   <si>
     <t>STD [n],Rs</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>SID [Rd],Rs</t>
   </si>
 </sst>
 </file>
@@ -1176,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1219,7 @@
       <c r="W3" s="37"/>
       <c r="X3" s="38"/>
       <c r="Z3" s="42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AA3" s="43"/>
       <c r="AB3" s="20"/>
@@ -1690,19 +1681,19 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H11" s="2">
         <v>2</v>
@@ -1768,7 +1759,7 @@
         <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>7</v>
@@ -1828,7 +1819,7 @@
         <v>22</v>
       </c>
       <c r="Z12" s="42" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AA12" s="43"/>
     </row>
@@ -2056,10 +2047,10 @@
         <v>22</v>
       </c>
       <c r="Z15" s="19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AA15" s="17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -2134,10 +2125,10 @@
         <v>22</v>
       </c>
       <c r="Z16" s="19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AA16" s="17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
@@ -2213,10 +2204,10 @@
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA17" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="AA17" s="17" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
@@ -2292,10 +2283,10 @@
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AA18" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
@@ -2377,13 +2368,13 @@
         <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>43</v>
@@ -2450,13 +2441,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>43</v>
@@ -2517,7 +2508,7 @@
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="42" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AA21" s="43"/>
     </row>
@@ -2669,7 +2660,7 @@
       </c>
       <c r="Y23" s="10"/>
       <c r="Z23" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AA23" s="26" t="s">
         <v>2</v>
@@ -2748,10 +2739,10 @@
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AA24" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
@@ -2827,10 +2818,10 @@
       </c>
       <c r="Y25" s="10"/>
       <c r="Z25" s="19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AA25" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
@@ -2906,10 +2897,10 @@
       </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AA26" s="17" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
@@ -2918,13 +2909,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>97</v>
@@ -2988,7 +2979,7 @@
         <v>45</v>
       </c>
       <c r="AA27" s="17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
@@ -3003,7 +2994,7 @@
         <v>115</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>97</v>
@@ -3067,7 +3058,7 @@
         <v>99</v>
       </c>
       <c r="AA28" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
@@ -3660,22 +3651,22 @@
         <v>92</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H37" s="2">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>33</v>

</xml_diff>